<commit_message>
update curve_carico, input_FM, main and config
</commit_message>
<xml_diff>
--- a/files/inputs_FM.xlsx
+++ b/files/inputs_FM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rollo\Tool\CACER simulator - DEVELOPER\CACER_simulator\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rsericerca-my.sharepoint.com/personal/rollo_rse-web_it/Documents/Desktop/CACER - public repo/CACER-simulator/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24024530-7E06-4182-B3E3-01B717966856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{24024530-7E06-4182-B3E3-01B717966856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE438CEC-8318-4C9F-9DF4-D2B70F6C423E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="741" activeTab="7" xr2:uid="{866B9CD4-6ADA-4356-B1C9-F1CC80F19CE1}"/>
   </bookViews>

</xml_diff>

<commit_message>
Fix bug cash flow
</commit_message>
<xml_diff>
--- a/files/inputs_FM.xlsx
+++ b/files/inputs_FM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rsericerca-my.sharepoint.com/personal/rollo_rse-web_it/Documents/Desktop/CACER - public repo/CACER-simulator/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{24024530-7E06-4182-B3E3-01B717966856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBA9A1F4-C475-4792-BA06-5B5D5971C4D5}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{24024530-7E06-4182-B3E3-01B717966856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DAA13D9-FC0B-4854-AEE2-EE40709E2157}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="741" activeTab="7" xr2:uid="{866B9CD4-6ADA-4356-B1C9-F1CC80F19CE1}"/>
   </bookViews>
@@ -3536,7 +3536,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>